<commit_message>
update test 1 / partly fixed test 2
</commit_message>
<xml_diff>
--- a/sample_data/2024/Q3/file_two_2024-09-30.xlsx
+++ b/sample_data/2024/Q3/file_two_2024-09-30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Desktop/File_checks/sample_data/2024/Q3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC30231-FDE4-314C-8E8F-D89403105FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA46CF54-B891-0640-8192-D5CD5121B8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1280" windowWidth="27640" windowHeight="16880" xr2:uid="{80B438F4-2709-A746-ADCD-824188E6626E}"/>
+    <workbookView xWindow="6060" yWindow="760" windowWidth="27640" windowHeight="16880" activeTab="1" xr2:uid="{80B438F4-2709-A746-ADCD-824188E6626E}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>a</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>test_row</t>
+  </si>
+  <si>
+    <t>col3</t>
+  </si>
+  <si>
+    <t>col5</t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4878BF-AB65-BB47-97C0-0C2689FD2CED}">
   <dimension ref="A4:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -598,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151B90E6-00AF-184B-9009-DB96519BD282}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,13 +618,13 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>